<commit_message>
Worked on dynamic export of chart svgs in local version of amCharts
</commit_message>
<xml_diff>
--- a/assets/ChartBuilder/public/Data/Backups/Catalyst/BUY/BUY.xlsx
+++ b/assets/ChartBuilder/public/Data/Backups/Catalyst/BUY/BUY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Dropbox (Catalyst Funds)\Marketing Team Files\Marketing Materials\AutoCharts&amp;Tables\Backup Files\Catalyst\BUY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrjak\Documents\GitHub\AutoCharts\assets\ChartBuilder\public\Data\Backups\Catalyst\BUY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E65FDCB-F088-42F0-8CBF-1DD0D4984A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCFFDF8-E69C-4DC1-AD2A-2913C567789C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="850" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="21600" windowHeight="11385" tabRatio="850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BUY Fact Sheet Backup" sheetId="3" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="BUY_EXPORT_PortfolioSector" sheetId="7" r:id="rId5"/>
     <sheet name="BUY_EXPORT_PerformanceTable" sheetId="8" r:id="rId6"/>
     <sheet name="BUY_EXPORT_PortCharacter" sheetId="9" r:id="rId7"/>
-    <sheet name="BUY_EXPORT_TopHoldings" sheetId="10" r:id="rId8"/>
-    <sheet name="BUY_EXPORT_PerformanceRisks" sheetId="11" r:id="rId9"/>
+    <sheet name="BUY_EXPORT_PerformanceRisks" sheetId="11" r:id="rId8"/>
+    <sheet name="BUY_EXPORT_TopHoldings" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="__FDS_HYPERLINK_TOGGLE_STATE__" hidden="1">"ON"</definedName>
@@ -1974,6 +1974,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2017,30 +2041,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2866,40 +2866,40 @@
   </sheetPr>
   <dimension ref="A1:X111"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="82" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="80" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="78" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="80" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="78" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="85" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="80" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="78" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="85" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.33203125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.28515625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2933,13 +2933,13 @@
       <c r="L1" s="4">
         <v>44196</v>
       </c>
-      <c r="S1" s="181" t="s">
+      <c r="S1" s="189" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="182"/>
-      <c r="U1" s="183"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="T1" s="190"/>
+      <c r="U1" s="191"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>41639</v>
       </c>
@@ -2970,13 +2970,13 @@
       <c r="O2" s="27"/>
       <c r="P2" s="27"/>
       <c r="Q2" s="9"/>
-      <c r="S2" s="184" t="s">
+      <c r="S2" s="192" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="185"/>
-      <c r="U2" s="186"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="T2" s="193"/>
+      <c r="U2" s="194"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>41670</v>
       </c>
@@ -3019,13 +3019,13 @@
       <c r="N3" s="28"/>
       <c r="O3" s="28"/>
       <c r="P3" s="28"/>
-      <c r="S3" s="187" t="s">
+      <c r="S3" s="195" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="188"/>
-      <c r="U3" s="189"/>
-    </row>
-    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T3" s="196"/>
+      <c r="U3" s="197"/>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>41698</v>
       </c>
@@ -3057,13 +3057,13 @@
       <c r="I4" s="83">
         <v>5.0700000000000002E-2</v>
       </c>
-      <c r="S4" s="190" t="s">
+      <c r="S4" s="198" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="191"/>
-      <c r="U4" s="192"/>
-    </row>
-    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T4" s="199"/>
+      <c r="U4" s="200"/>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>41729</v>
       </c>
@@ -3095,16 +3095,16 @@
       <c r="I5" s="83">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="K5" s="178" t="s">
+      <c r="K5" s="186" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="179"/>
-      <c r="M5" s="179"/>
-      <c r="N5" s="179"/>
-      <c r="O5" s="179"/>
-      <c r="P5" s="180"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="L5" s="187"/>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="188"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>41759</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>41790</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>15132.649940973706</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>41820</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>15132.649940973706</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>41851</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>13557.833083402626</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>41882</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>10296.646548436947</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>41912</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>41943</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>16982.213367869452</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>41973</v>
       </c>
@@ -3626,7 +3626,7 @@
       <c r="W13" s="99"/>
       <c r="X13" s="99"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>42004</v>
       </c>
@@ -3681,8 +3681,8 @@
         <f>X23*100</f>
         <v>5.99</v>
       </c>
-      <c r="S14" s="199"/>
-      <c r="T14" s="200"/>
+      <c r="S14" s="184"/>
+      <c r="T14" s="185"/>
       <c r="U14" s="100" t="str">
         <f>U6</f>
         <v>BUYIX</v>
@@ -3700,7 +3700,7 @@
         <v>Mid-Cap Blend</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>42035</v>
       </c>
@@ -3755,11 +3755,11 @@
         <f>X25*100</f>
         <v>5.2</v>
       </c>
-      <c r="S15" s="195" t="str">
+      <c r="S15" s="180" t="str">
         <f>S7</f>
         <v>YTD</v>
       </c>
-      <c r="T15" s="196"/>
+      <c r="T15" s="181"/>
       <c r="U15" s="165">
         <v>2.5100000000000001E-2</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>0.1239</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>42063</v>
       </c>
@@ -3826,11 +3826,11 @@
         <f>X29*100</f>
         <v>7.8589846324937707</v>
       </c>
-      <c r="S16" s="195" t="str">
+      <c r="S16" s="180" t="str">
         <f>S8</f>
         <v>1YR</v>
       </c>
-      <c r="T16" s="196"/>
+      <c r="T16" s="181"/>
       <c r="U16" s="103">
         <f>U12/U8-1</f>
         <v>2.5118896108245803E-2</v>
@@ -3847,7 +3847,7 @@
         <v>0.1239</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>42094</v>
       </c>
@@ -3902,11 +3902,11 @@
         <v>12.92</v>
       </c>
       <c r="Q17" s="9"/>
-      <c r="S17" s="195" t="str">
+      <c r="S17" s="180" t="str">
         <f>S9</f>
         <v>3YR</v>
       </c>
-      <c r="T17" s="196"/>
+      <c r="T17" s="181"/>
       <c r="U17" s="103">
         <f>(U12/U9)^(1/3)-1</f>
         <v>3.7648641636830238E-2</v>
@@ -3923,7 +3923,7 @@
         <v>8.2699999999999996E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>42124</v>
       </c>
@@ -3979,11 +3979,11 @@
         <v>12.760328113022968</v>
       </c>
       <c r="Q18" s="9"/>
-      <c r="S18" s="193" t="str">
+      <c r="S18" s="178" t="str">
         <f>S10</f>
         <v>5YR</v>
       </c>
-      <c r="T18" s="194"/>
+      <c r="T18" s="179"/>
       <c r="U18" s="103">
         <f>(U12/U10)^(1/5)-1</f>
         <v>9.0339593209082913E-2</v>
@@ -4000,7 +4000,7 @@
         <v>0.1108</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>42155</v>
       </c>
@@ -4056,10 +4056,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="Q19" s="9"/>
-      <c r="S19" s="195" t="s">
+      <c r="S19" s="180" t="s">
         <v>45</v>
       </c>
-      <c r="T19" s="196"/>
+      <c r="T19" s="181"/>
       <c r="U19" s="103">
         <f>($U$12-U11)/U11</f>
         <v>0.53039999999999998</v>
@@ -4077,7 +4077,7 @@
         <v>0.6982213367869452</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>42185</v>
       </c>
@@ -4116,10 +4116,10 @@
       <c r="O20" s="61"/>
       <c r="P20" s="77"/>
       <c r="Q20" s="9"/>
-      <c r="S20" s="197" t="s">
+      <c r="S20" s="182" t="s">
         <v>9</v>
       </c>
-      <c r="T20" s="198"/>
+      <c r="T20" s="183"/>
       <c r="U20" s="122">
         <f>(1+U19)^(12/L3)-1</f>
         <v>6.2675598163236312E-2</v>
@@ -4136,7 +4136,7 @@
         <v>7.8589846324937707E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>42216</v>
       </c>
@@ -4179,7 +4179,7 @@
       <c r="W21" s="99"/>
       <c r="X21" s="99"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>42247</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>42277</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>5.9900000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>42308</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>42338</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>42369</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>6.2675598163236312E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>42400</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>0.12920000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>42429</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>0.12760328113022967</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>42460</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>7.8589846324937707E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>42490</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>7.8E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>42521</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>-4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>42551</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>0.1414</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>42582</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>0.1593</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>42613</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>-0.1115</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>42643</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>0.2621</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>42674</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>0.1239</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>42704</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>6.6400000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>42735</v>
       </c>
@@ -5155,7 +5155,7 @@
       <c r="L38" s="168"/>
       <c r="M38" s="7"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>42766</v>
       </c>
@@ -5192,7 +5192,7 @@
       <c r="L39" s="32"/>
       <c r="N39" s="31"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>42794</v>
       </c>
@@ -5233,7 +5233,7 @@
       <c r="Q40" s="169"/>
       <c r="R40"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>42825</v>
       </c>
@@ -5274,7 +5274,7 @@
       <c r="Q41" s="169"/>
       <c r="R41" s="169"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="117" t="s">
         <v>56</v>
       </c>
@@ -5315,7 +5315,7 @@
       <c r="Q42" s="169"/>
       <c r="R42" s="169"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="117" t="s">
         <v>57</v>
       </c>
@@ -5356,7 +5356,7 @@
       <c r="Q43" s="169"/>
       <c r="R43" s="169"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="117" t="s">
         <v>58</v>
       </c>
@@ -5397,7 +5397,7 @@
       <c r="Q44" s="169"/>
       <c r="R44" s="169"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>42947</v>
       </c>
@@ -5438,7 +5438,7 @@
       <c r="Q45" s="169"/>
       <c r="R45" s="169"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>42978</v>
       </c>
@@ -5479,7 +5479,7 @@
       <c r="Q46" s="169"/>
       <c r="R46" s="169"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43008</v>
       </c>
@@ -5520,7 +5520,7 @@
       <c r="Q47" s="169"/>
       <c r="R47" s="169"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <f>EOMONTH(A47,1)</f>
         <v>43039</v>
@@ -5563,7 +5563,7 @@
       <c r="Q48" s="169"/>
       <c r="R48" s="169"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <f t="shared" ref="A49:A86" si="15">EOMONTH(A48,1)</f>
         <v>43069</v>
@@ -5606,7 +5606,7 @@
       <c r="Q49" s="169"/>
       <c r="R49" s="169"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <f t="shared" si="15"/>
         <v>43100</v>
@@ -5649,7 +5649,7 @@
       <c r="Q50" s="169"/>
       <c r="R50" s="169"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <f t="shared" si="15"/>
         <v>43131</v>
@@ -5692,7 +5692,7 @@
       <c r="Q51" s="169"/>
       <c r="R51" s="169"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <f t="shared" si="15"/>
         <v>43159</v>
@@ -5735,7 +5735,7 @@
       <c r="Q52"/>
       <c r="R52"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <f t="shared" si="15"/>
         <v>43190</v>
@@ -5774,7 +5774,7 @@
       <c r="M53" s="31"/>
       <c r="N53" s="31"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <f t="shared" si="15"/>
         <v>43220</v>
@@ -5813,7 +5813,7 @@
       <c r="M54" s="31"/>
       <c r="N54" s="31"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <f t="shared" si="15"/>
         <v>43251</v>
@@ -5852,7 +5852,7 @@
       <c r="M55" s="31"/>
       <c r="N55" s="31"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <f t="shared" si="15"/>
         <v>43281</v>
@@ -5891,7 +5891,7 @@
       <c r="M56" s="31"/>
       <c r="N56" s="31"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <f t="shared" si="15"/>
         <v>43312</v>
@@ -5930,7 +5930,7 @@
       <c r="M57" s="31"/>
       <c r="N57" s="31"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <f t="shared" si="15"/>
         <v>43343</v>
@@ -5969,7 +5969,7 @@
       <c r="M58" s="31"/>
       <c r="N58" s="31"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <f t="shared" si="15"/>
         <v>43373</v>
@@ -6008,7 +6008,7 @@
       <c r="M59" s="31"/>
       <c r="N59" s="31"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <f t="shared" si="15"/>
         <v>43404</v>
@@ -6047,7 +6047,7 @@
       <c r="M60" s="31"/>
       <c r="N60" s="31"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <f t="shared" si="15"/>
         <v>43434</v>
@@ -6086,7 +6086,7 @@
       <c r="M61" s="31"/>
       <c r="N61" s="31"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <f t="shared" si="15"/>
         <v>43465</v>
@@ -6125,7 +6125,7 @@
       <c r="M62" s="31"/>
       <c r="N62" s="31"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <f t="shared" si="15"/>
         <v>43496</v>
@@ -6164,7 +6164,7 @@
       <c r="M63" s="31"/>
       <c r="N63" s="31"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <f t="shared" si="15"/>
         <v>43524</v>
@@ -6203,7 +6203,7 @@
       <c r="M64" s="31"/>
       <c r="N64" s="31"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <f t="shared" si="15"/>
         <v>43555</v>
@@ -6242,7 +6242,7 @@
       <c r="M65" s="31"/>
       <c r="N65" s="31"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <f t="shared" si="15"/>
         <v>43585</v>
@@ -6281,7 +6281,7 @@
       <c r="M66" s="31"/>
       <c r="N66" s="31"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <f t="shared" si="15"/>
         <v>43616</v>
@@ -6320,7 +6320,7 @@
       <c r="M67" s="31"/>
       <c r="N67" s="31"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <f t="shared" si="15"/>
         <v>43646</v>
@@ -6359,7 +6359,7 @@
       <c r="M68" s="31"/>
       <c r="N68" s="31"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <f t="shared" si="15"/>
         <v>43677</v>
@@ -6398,7 +6398,7 @@
       <c r="M69" s="31"/>
       <c r="N69" s="31"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <f t="shared" si="15"/>
         <v>43708</v>
@@ -6437,7 +6437,7 @@
       <c r="M70" s="31"/>
       <c r="N70" s="31"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <f t="shared" si="15"/>
         <v>43738</v>
@@ -6476,7 +6476,7 @@
       <c r="M71" s="31"/>
       <c r="N71" s="31"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <f t="shared" si="15"/>
         <v>43769</v>
@@ -6515,7 +6515,7 @@
       <c r="M72" s="31"/>
       <c r="N72" s="31"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <f t="shared" si="15"/>
         <v>43799</v>
@@ -6554,7 +6554,7 @@
       <c r="M73" s="31"/>
       <c r="N73" s="31"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <f t="shared" si="15"/>
         <v>43830</v>
@@ -6593,7 +6593,7 @@
       <c r="M74" s="31"/>
       <c r="N74" s="31"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <f t="shared" si="15"/>
         <v>43861</v>
@@ -6632,7 +6632,7 @@
       <c r="M75" s="31"/>
       <c r="N75" s="31"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <f t="shared" si="15"/>
         <v>43890</v>
@@ -6671,7 +6671,7 @@
       <c r="M76" s="31"/>
       <c r="N76" s="31"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <f t="shared" si="15"/>
         <v>43921</v>
@@ -6710,7 +6710,7 @@
       <c r="M77" s="31"/>
       <c r="N77" s="31"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <f t="shared" si="15"/>
         <v>43951</v>
@@ -6749,7 +6749,7 @@
       <c r="M78" s="31"/>
       <c r="N78" s="31"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <f t="shared" si="15"/>
         <v>43982</v>
@@ -6788,7 +6788,7 @@
       <c r="M79" s="31"/>
       <c r="N79" s="31"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <f t="shared" si="15"/>
         <v>44012</v>
@@ -6827,7 +6827,7 @@
       <c r="M80" s="31"/>
       <c r="N80" s="31"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <f t="shared" si="15"/>
         <v>44043</v>
@@ -6866,7 +6866,7 @@
       <c r="M81" s="31"/>
       <c r="N81" s="31"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <f t="shared" si="15"/>
         <v>44074</v>
@@ -6905,7 +6905,7 @@
       <c r="M82" s="31"/>
       <c r="N82" s="31"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <f t="shared" si="15"/>
         <v>44104</v>
@@ -6944,7 +6944,7 @@
       <c r="M83" s="31"/>
       <c r="N83" s="31"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <f t="shared" si="15"/>
         <v>44135</v>
@@ -6983,7 +6983,7 @@
       <c r="M84" s="31"/>
       <c r="N84" s="31"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
         <f t="shared" si="15"/>
         <v>44165</v>
@@ -7022,7 +7022,7 @@
       <c r="M85" s="31"/>
       <c r="N85" s="31"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
         <f t="shared" si="15"/>
         <v>44196</v>
@@ -7061,7 +7061,7 @@
       <c r="M86" s="31"/>
       <c r="N86" s="31"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E87" s="81"/>
       <c r="F87" s="81"/>
       <c r="G87" s="81"/>
@@ -7072,7 +7072,7 @@
       <c r="M87" s="31"/>
       <c r="N87" s="31"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E88" s="81"/>
       <c r="F88" s="81"/>
       <c r="G88" s="81"/>
@@ -7083,7 +7083,7 @@
       <c r="M88" s="31"/>
       <c r="N88" s="31"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E89" s="81"/>
       <c r="F89" s="81"/>
       <c r="G89" s="81"/>
@@ -7094,7 +7094,7 @@
       <c r="M89" s="31"/>
       <c r="N89" s="31"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E90" s="81"/>
       <c r="F90" s="81"/>
       <c r="G90" s="81"/>
@@ -7105,7 +7105,7 @@
       <c r="M90" s="31"/>
       <c r="N90" s="31"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E91" s="81"/>
       <c r="F91" s="81"/>
       <c r="G91" s="81"/>
@@ -7116,7 +7116,7 @@
       <c r="M91" s="31"/>
       <c r="N91" s="31"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E92" s="81"/>
       <c r="F92" s="81"/>
       <c r="G92" s="81"/>
@@ -7127,7 +7127,7 @@
       <c r="M92" s="31"/>
       <c r="N92" s="31"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E93" s="81"/>
       <c r="F93" s="81"/>
       <c r="G93" s="81"/>
@@ -7138,7 +7138,7 @@
       <c r="M93" s="31"/>
       <c r="N93" s="31"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E94" s="81"/>
       <c r="F94" s="81"/>
       <c r="G94" s="81"/>
@@ -7149,7 +7149,7 @@
       <c r="M94" s="31"/>
       <c r="N94" s="31"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E95" s="81"/>
       <c r="F95" s="81"/>
       <c r="G95" s="81"/>
@@ -7160,7 +7160,7 @@
       <c r="M95" s="31"/>
       <c r="N95" s="31"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E96" s="81"/>
       <c r="F96" s="81"/>
       <c r="G96" s="81"/>
@@ -7171,7 +7171,7 @@
       <c r="M96" s="31"/>
       <c r="N96" s="31"/>
     </row>
-    <row r="97" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E97" s="81"/>
       <c r="F97" s="81"/>
       <c r="G97" s="81"/>
@@ -7182,7 +7182,7 @@
       <c r="M97" s="31"/>
       <c r="N97" s="31"/>
     </row>
-    <row r="98" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E98" s="81"/>
       <c r="F98" s="81"/>
       <c r="G98" s="81"/>
@@ -7193,7 +7193,7 @@
       <c r="M98" s="31"/>
       <c r="N98" s="31"/>
     </row>
-    <row r="99" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E99" s="81"/>
       <c r="F99" s="81"/>
       <c r="G99" s="81"/>
@@ -7204,7 +7204,7 @@
       <c r="M99" s="31"/>
       <c r="N99" s="31"/>
     </row>
-    <row r="100" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E100" s="81"/>
       <c r="F100" s="81"/>
       <c r="G100" s="81"/>
@@ -7215,7 +7215,7 @@
       <c r="M100" s="31"/>
       <c r="N100" s="31"/>
     </row>
-    <row r="101" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E101" s="81"/>
       <c r="F101" s="81"/>
       <c r="G101" s="81"/>
@@ -7226,7 +7226,7 @@
       <c r="M101" s="31"/>
       <c r="N101" s="31"/>
     </row>
-    <row r="102" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E102" s="81"/>
       <c r="F102" s="81"/>
       <c r="G102" s="81"/>
@@ -7237,7 +7237,7 @@
       <c r="M102" s="31"/>
       <c r="N102" s="31"/>
     </row>
-    <row r="103" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E103" s="81"/>
       <c r="F103" s="81"/>
       <c r="G103" s="81"/>
@@ -7248,7 +7248,7 @@
       <c r="M103" s="31"/>
       <c r="N103" s="31"/>
     </row>
-    <row r="104" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E104" s="81"/>
       <c r="F104" s="81"/>
       <c r="G104" s="81"/>
@@ -7259,7 +7259,7 @@
       <c r="M104" s="31"/>
       <c r="N104" s="31"/>
     </row>
-    <row r="105" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E105" s="81"/>
       <c r="F105" s="81"/>
       <c r="G105" s="81"/>
@@ -7270,7 +7270,7 @@
       <c r="M105" s="31"/>
       <c r="N105" s="31"/>
     </row>
-    <row r="106" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E106" s="81"/>
       <c r="F106" s="81"/>
       <c r="G106" s="81"/>
@@ -7281,7 +7281,7 @@
       <c r="M106" s="31"/>
       <c r="N106" s="31"/>
     </row>
-    <row r="107" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E107" s="81"/>
       <c r="F107" s="81"/>
       <c r="G107" s="81"/>
@@ -7292,7 +7292,7 @@
       <c r="M107" s="31"/>
       <c r="N107" s="31"/>
     </row>
-    <row r="108" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E108" s="81"/>
       <c r="F108" s="81"/>
       <c r="G108" s="81"/>
@@ -7303,7 +7303,7 @@
       <c r="M108" s="31"/>
       <c r="N108" s="31"/>
     </row>
-    <row r="109" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E109" s="81"/>
       <c r="F109" s="81"/>
       <c r="G109" s="81"/>
@@ -7314,7 +7314,7 @@
       <c r="M109" s="31"/>
       <c r="N109" s="31"/>
     </row>
-    <row r="110" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E110" s="81"/>
       <c r="F110" s="81"/>
       <c r="G110" s="81"/>
@@ -7325,7 +7325,7 @@
       <c r="M110" s="31"/>
       <c r="N110" s="31"/>
     </row>
-    <row r="111" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E111" s="81"/>
       <c r="F111" s="81"/>
       <c r="G111" s="81"/>
@@ -7338,6 +7338,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S4:U4"/>
     <mergeCell ref="S18:T18"/>
     <mergeCell ref="S19:T19"/>
     <mergeCell ref="S20:T20"/>
@@ -7345,11 +7350,6 @@
     <mergeCell ref="S15:T15"/>
     <mergeCell ref="S16:T16"/>
     <mergeCell ref="S17:T17"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -7367,38 +7367,38 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="23.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="23.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="8" style="5" customWidth="1"/>
     <col min="4" max="4" width="3" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="7"/>
-    <col min="7" max="7" width="4.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="2"/>
+    <col min="5" max="5" width="19.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="7"/>
+    <col min="7" max="7" width="4.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="178" t="s">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="186" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
-      <c r="H2" s="179"/>
-      <c r="I2" s="180"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="188"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="53"/>
       <c r="C3" s="45"/>
       <c r="I3" s="54"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="201" t="s">
         <v>49</v>
       </c>
@@ -7412,7 +7412,7 @@
       </c>
       <c r="I4" s="57"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
         <v>103</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>0.3685471670549067</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="58" t="s">
         <v>104</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>0.20962292124663828</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="58" t="s">
         <v>105</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>0.12004675685711351</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="58" t="s">
         <v>106</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>0.11977017521717757</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
       <c r="E9" s="46" t="s">
         <v>108</v>
@@ -7507,7 +7507,7 @@
         <v>9.1352095488908713E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
       <c r="C10" s="60"/>
       <c r="E10" s="46" t="s">
@@ -7523,7 +7523,7 @@
         <v>5.1276618056670747E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" s="60"/>
       <c r="E11" s="46" t="s">
@@ -7539,7 +7539,7 @@
         <v>3.9277775009029202E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="E12" s="46" t="s">
         <v>178</v>
@@ -7554,7 +7554,7 @@
         <v>1.0649106955527131E-4</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
       <c r="E13" s="46" t="s">
         <v>179</v>
@@ -7565,7 +7565,7 @@
       <c r="H13" s="46"/>
       <c r="I13" s="59"/>
     </row>
-    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="24"/>
       <c r="C14" s="61"/>
       <c r="D14" s="61"/>
@@ -7579,42 +7579,42 @@
       <c r="H14" s="62"/>
       <c r="I14" s="163"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G15" s="52"/>
       <c r="I15" s="127"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F16" s="2"/>
       <c r="I16" s="127"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
     </row>
   </sheetData>
@@ -7635,36 +7635,36 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="21.5546875" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.44140625" customWidth="1"/>
-    <col min="17" max="17" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="38.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:17" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="38.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:17" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="152" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="152" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="152" t="s">
         <v>181</v>
       </c>
@@ -7680,7 +7680,7 @@
       <c r="P5" s="35"/>
       <c r="Q5" s="35"/>
     </row>
-    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="152" t="s">
         <v>22</v>
       </c>
@@ -7696,7 +7696,7 @@
       <c r="P6" s="35"/>
       <c r="Q6" s="35"/>
     </row>
-    <row r="7" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="149" t="s">
         <v>24</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="150" t="s">
         <v>60</v>
       </c>
@@ -7758,7 +7758,7 @@
       <c r="P8" s="35"/>
       <c r="Q8" s="35"/>
     </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="150" t="s">
         <v>109</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>0.3685471670549067</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="137" t="s">
         <v>69</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>0.20962292124663828</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="137" t="s">
         <v>81</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>0.12004675685711351</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="137" t="s">
         <v>72</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>0.11977017521717757</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="137" t="s">
         <v>122</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>9.1352095488908713E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="137" t="s">
         <v>114</v>
       </c>
@@ -8021,7 +8021,7 @@
         <v>5.1276618056670747E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="137" t="s">
         <v>112</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>3.9277775009029202E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="137" t="s">
         <v>66</v>
       </c>
@@ -8117,7 +8117,7 @@
         <v>1.0649106955527131E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="137" t="s">
         <v>150</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="137" t="s">
         <v>130</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="137" t="s">
         <v>110</v>
       </c>
@@ -8261,7 +8261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="137" t="s">
         <v>118</v>
       </c>
@@ -8307,7 +8307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="137" t="s">
         <v>157</v>
       </c>
@@ -8349,7 +8349,7 @@
       <c r="P21" s="35"/>
       <c r="Q21" s="35"/>
     </row>
-    <row r="22" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="137" t="s">
         <v>154</v>
       </c>
@@ -8391,7 +8391,7 @@
       <c r="P22" s="35"/>
       <c r="Q22" s="35"/>
     </row>
-    <row r="23" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="137" t="s">
         <v>94</v>
       </c>
@@ -8433,7 +8433,7 @@
       <c r="P23" s="35"/>
       <c r="Q23" s="35"/>
     </row>
-    <row r="24" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="137" t="s">
         <v>120</v>
       </c>
@@ -8475,7 +8475,7 @@
       <c r="P24" s="35"/>
       <c r="Q24" s="35"/>
     </row>
-    <row r="25" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="137" t="s">
         <v>128</v>
       </c>
@@ -8517,7 +8517,7 @@
       <c r="P25" s="35"/>
       <c r="Q25" s="35"/>
     </row>
-    <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="137" t="s">
         <v>92</v>
       </c>
@@ -8559,7 +8559,7 @@
       <c r="P26" s="35"/>
       <c r="Q26" s="35"/>
     </row>
-    <row r="27" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="137" t="s">
         <v>126</v>
       </c>
@@ -8601,7 +8601,7 @@
       <c r="P27" s="35"/>
       <c r="Q27" s="35"/>
     </row>
-    <row r="28" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="137" t="s">
         <v>90</v>
       </c>
@@ -8643,7 +8643,7 @@
       <c r="P28" s="35"/>
       <c r="Q28" s="35"/>
     </row>
-    <row r="29" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="137" t="s">
         <v>184</v>
       </c>
@@ -8685,7 +8685,7 @@
       <c r="P29" s="35"/>
       <c r="Q29" s="35"/>
     </row>
-    <row r="30" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="137" t="s">
         <v>75</v>
       </c>
@@ -8727,7 +8727,7 @@
       <c r="P30" s="35"/>
       <c r="Q30" s="35"/>
     </row>
-    <row r="31" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="137" t="s">
         <v>188</v>
       </c>
@@ -8769,7 +8769,7 @@
       <c r="P31" s="35"/>
       <c r="Q31" s="35"/>
     </row>
-    <row r="32" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="137" t="s">
         <v>132</v>
       </c>
@@ -8811,7 +8811,7 @@
       <c r="P32" s="35"/>
       <c r="Q32" s="35"/>
     </row>
-    <row r="33" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="137" t="s">
         <v>168</v>
       </c>
@@ -8853,7 +8853,7 @@
       <c r="P33" s="35"/>
       <c r="Q33" s="35"/>
     </row>
-    <row r="34" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="137" t="s">
         <v>164</v>
       </c>
@@ -8895,7 +8895,7 @@
       <c r="P34" s="35"/>
       <c r="Q34" s="35"/>
     </row>
-    <row r="35" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="137" t="s">
         <v>171</v>
       </c>
@@ -8937,7 +8937,7 @@
       <c r="P35" s="35"/>
       <c r="Q35" s="35"/>
     </row>
-    <row r="36" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="137" t="s">
         <v>124</v>
       </c>
@@ -8979,7 +8979,7 @@
       <c r="P36" s="35"/>
       <c r="Q36" s="35"/>
     </row>
-    <row r="37" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="137" t="s">
         <v>79</v>
       </c>
@@ -9021,7 +9021,7 @@
       <c r="P37" s="35"/>
       <c r="Q37" s="35"/>
     </row>
-    <row r="38" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="137" t="s">
         <v>191</v>
       </c>
@@ -9063,7 +9063,7 @@
       <c r="P38" s="35"/>
       <c r="Q38" s="35"/>
     </row>
-    <row r="39" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="137" t="s">
         <v>77</v>
       </c>
@@ -9105,7 +9105,7 @@
       <c r="P39" s="35"/>
       <c r="Q39" s="35"/>
     </row>
-    <row r="40" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="137" t="s">
         <v>194</v>
       </c>
@@ -9147,7 +9147,7 @@
       <c r="P40" s="35"/>
       <c r="Q40" s="35"/>
     </row>
-    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="137" t="s">
         <v>116</v>
       </c>
@@ -9189,7 +9189,7 @@
       <c r="P41" s="35"/>
       <c r="Q41" s="35"/>
     </row>
-    <row r="42" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="137" t="s">
         <v>134</v>
       </c>
@@ -9229,7 +9229,7 @@
       </c>
       <c r="N42" s="39"/>
     </row>
-    <row r="43" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="151" t="s">
         <v>136</v>
       </c>
@@ -9245,7 +9245,7 @@
       </c>
       <c r="M43" s="176"/>
     </row>
-    <row r="44" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="150" t="s">
         <v>197</v>
       </c>
@@ -9257,7 +9257,7 @@
       <c r="G44" s="137"/>
       <c r="M44" s="176"/>
     </row>
-    <row r="45" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="137" t="s">
         <v>198</v>
       </c>
@@ -9287,7 +9287,7 @@
         <v>1.0649106955527131E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="151" t="s">
         <v>200</v>
       </c>
@@ -9302,7 +9302,7 @@
         <v>1107.7</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="151" t="s">
         <v>61</v>
       </c>
@@ -9317,7 +9317,7 @@
         <v>10401811.199999999</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="152"/>
       <c r="B48" s="152"/>
       <c r="C48" s="152"/>
@@ -9326,7 +9326,7 @@
       <c r="F48" s="137"/>
       <c r="G48" s="137"/>
     </row>
-    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="151" t="s">
         <v>61</v>
       </c>
@@ -9341,26 +9341,26 @@
         <v>10401811.199999999</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.25" footer="0.25"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -9374,7 +9374,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4767E4B-C7EC-42BD-9E21-F35DD6BD63B3}">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -9382,12 +9382,12 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9403,7 +9403,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>'BUY Fact Sheet Backup'!N30</f>
         <v>2014</v>
@@ -9420,7 +9420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>'BUY Fact Sheet Backup'!N31</f>
         <v>2015</v>
@@ -9437,7 +9437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>'BUY Fact Sheet Backup'!N32</f>
         <v>2016</v>
@@ -9454,7 +9454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>'BUY Fact Sheet Backup'!N33</f>
         <v>2017</v>
@@ -9471,7 +9471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>'BUY Fact Sheet Backup'!N34</f>
         <v>2018</v>
@@ -9488,7 +9488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>'BUY Fact Sheet Backup'!N35</f>
         <v>2019</v>
@@ -9505,7 +9505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -9521,10 +9521,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="153"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="153"/>
     </row>
   </sheetData>
@@ -9536,19 +9536,21 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275A7FD0-31DE-42A4-96E8-F349AC623B4A}">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -9559,7 +9561,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'BUY Portfolio'!H5</f>
         <v>Information Technology</v>
@@ -9572,7 +9574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'BUY Portfolio'!H6</f>
         <v>Health Care</v>
@@ -9585,7 +9587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'BUY Portfolio'!H7</f>
         <v>Consumer Discretionary</v>
@@ -9598,7 +9600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'BUY Portfolio'!H8</f>
         <v>Industrials</v>
@@ -9611,7 +9613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>'BUY Portfolio'!H9</f>
         <v>Financials</v>
@@ -9624,7 +9626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>'BUY Portfolio'!H10</f>
         <v>Consumer Staples</v>
@@ -9637,7 +9639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'BUY Portfolio'!H11</f>
         <v>Communication Services</v>
@@ -9650,25 +9652,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="154"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="154"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="154"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="154"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="154"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="154"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="154"/>
     </row>
   </sheetData>
@@ -9679,22 +9681,22 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1A2606-18BD-43F5-B41C-691CB4392628}">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.109375" style="156"/>
-    <col min="6" max="6" width="15.6640625" style="156" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="156"/>
+    <col min="6" max="6" width="15.7109375" style="156" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="155" t="str">
         <f>'BUY Fact Sheet Backup'!S22</f>
         <v>Share Class/Benchmark</v>
@@ -9722,7 +9724,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="155" t="s">
         <v>48</v>
       </c>
@@ -9750,7 +9752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="155" t="s">
         <v>42</v>
       </c>
@@ -9778,7 +9780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="155" t="s">
         <v>43</v>
       </c>
@@ -9806,7 +9808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="155" t="s">
         <v>62</v>
       </c>
@@ -9834,7 +9836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="155" t="s">
         <v>137</v>
       </c>
@@ -9862,7 +9864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="155" t="s">
         <v>138</v>
       </c>
@@ -9890,7 +9892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="155" t="s">
         <v>44</v>
       </c>
@@ -9918,7 +9920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="155"/>
     </row>
   </sheetData>
@@ -9930,20 +9932,20 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C19FE0-1575-4562-9EB5-F6AB40F72705}">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -9954,7 +9956,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -9966,7 +9968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -9978,7 +9980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -9990,7 +9992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -10008,158 +10010,83 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05316E0F-C3C1-44AD-B94F-F231B1ED2A12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD8AEA4-CA22-41AE-A1A3-10A3A98C6279}">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>84</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f>'BUY Portfolio'!E5</f>
-        <v>Apple Inc</v>
-      </c>
-      <c r="B2" s="154">
-        <f>'BUY Portfolio'!F5*100</f>
-        <v>8.5</v>
-      </c>
-      <c r="C2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="156">
+        <f>'BUY Fact Sheet Backup'!L8*100</f>
+        <v>-1.0338375846980039</v>
+      </c>
+      <c r="C2" t="str">
+        <f>'BUY Fact Sheet Backup'!M8</f>
+        <v>-</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>'BUY Portfolio'!E6</f>
-        <v>Qorvo Inc</v>
-      </c>
-      <c r="B3" s="154">
-        <f>'BUY Portfolio'!F6*100</f>
-        <v>7.5</v>
-      </c>
-      <c r="C3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="156">
+        <f>'BUY Fact Sheet Backup'!L9</f>
+        <v>0.92839221597015387</v>
+      </c>
+      <c r="C3" t="str">
+        <f>'BUY Fact Sheet Backup'!M9</f>
+        <v>-</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f>'BUY Portfolio'!E7</f>
-        <v>Pool Corp</v>
-      </c>
-      <c r="B4" s="154">
-        <f>'BUY Portfolio'!F7*100</f>
-        <v>5.8999999999999995</v>
-      </c>
-      <c r="C4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="156">
+        <f>'BUY Fact Sheet Backup'!L10</f>
+        <v>0.91118483576664933</v>
+      </c>
+      <c r="C4" t="str">
+        <f>'BUY Fact Sheet Backup'!M10</f>
+        <v>-</v>
+      </c>
+      <c r="D4">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>'BUY Portfolio'!E8</f>
-        <v>Triton International Ltd/Bermu</v>
-      </c>
-      <c r="B5" s="154">
-        <f>'BUY Portfolio'!F8*100</f>
-        <v>4.7</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f>'BUY Portfolio'!E9</f>
-        <v>West Pharmaceutical Services I</v>
-      </c>
-      <c r="B6" s="154">
-        <f>'BUY Portfolio'!F9*100</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f>'BUY Portfolio'!E10</f>
-        <v>GoDaddy Inc</v>
-      </c>
-      <c r="B7" s="154">
-        <f>'BUY Portfolio'!F10*100</f>
-        <v>4.3999999999999995</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f>'BUY Portfolio'!E11</f>
-        <v>Microsoft Corp</v>
-      </c>
-      <c r="B8" s="154">
-        <f>'BUY Portfolio'!F11*100</f>
-        <v>4.2</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f>'BUY Portfolio'!E12</f>
-        <v>Mr Cooper Group Inc</v>
-      </c>
-      <c r="B9" s="154">
-        <f>'BUY Portfolio'!F12*100</f>
-        <v>3.9</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f>'BUY Portfolio'!E13</f>
-        <v>Providence Service Corp/The</v>
-      </c>
-      <c r="B10" s="154">
-        <f>'BUY Portfolio'!F13*100</f>
-        <v>3.6999999999999997</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f>'BUY Portfolio'!E14</f>
-        <v>Masimo Corp</v>
-      </c>
-      <c r="B11" s="154">
-        <f>'BUY Portfolio'!F14*100</f>
-        <v>3.5999999999999996</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -10168,81 +10095,160 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD8AEA4-CA22-41AE-A1A3-10A3A98C6279}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05316E0F-C3C1-44AD-B94F-F231B1ED2A12}">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>84</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" s="156">
-        <f>'BUY Fact Sheet Backup'!L8*100</f>
-        <v>-1.0338375846980039</v>
-      </c>
-      <c r="C2" t="str">
-        <f>'BUY Fact Sheet Backup'!M8</f>
-        <v>-</v>
-      </c>
-      <c r="D2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>'BUY Portfolio'!E5</f>
+        <v>Apple Inc</v>
+      </c>
+      <c r="B2" s="154">
+        <f>'BUY Portfolio'!F5*100</f>
+        <v>8.5</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="156">
-        <f>'BUY Fact Sheet Backup'!L9</f>
-        <v>0.92839221597015387</v>
-      </c>
-      <c r="C3" t="str">
-        <f>'BUY Fact Sheet Backup'!M9</f>
-        <v>-</v>
-      </c>
-      <c r="D3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>'BUY Portfolio'!E6</f>
+        <v>Qorvo Inc</v>
+      </c>
+      <c r="B3" s="154">
+        <f>'BUY Portfolio'!F6*100</f>
+        <v>7.5</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B4" s="156">
-        <f>'BUY Fact Sheet Backup'!L10</f>
-        <v>0.91118483576664933</v>
-      </c>
-      <c r="C4" t="str">
-        <f>'BUY Fact Sheet Backup'!M10</f>
-        <v>-</v>
-      </c>
-      <c r="D4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>'BUY Portfolio'!E7</f>
+        <v>Pool Corp</v>
+      </c>
+      <c r="B4" s="154">
+        <f>'BUY Portfolio'!F7*100</f>
+        <v>5.8999999999999995</v>
+      </c>
+      <c r="C4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>'BUY Portfolio'!E8</f>
+        <v>Triton International Ltd/Bermu</v>
+      </c>
+      <c r="B5" s="154">
+        <f>'BUY Portfolio'!F8*100</f>
+        <v>4.7</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>'BUY Portfolio'!E9</f>
+        <v>West Pharmaceutical Services I</v>
+      </c>
+      <c r="B6" s="154">
+        <f>'BUY Portfolio'!F9*100</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>'BUY Portfolio'!E10</f>
+        <v>GoDaddy Inc</v>
+      </c>
+      <c r="B7" s="154">
+        <f>'BUY Portfolio'!F10*100</f>
+        <v>4.3999999999999995</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>'BUY Portfolio'!E11</f>
+        <v>Microsoft Corp</v>
+      </c>
+      <c r="B8" s="154">
+        <f>'BUY Portfolio'!F11*100</f>
+        <v>4.2</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>'BUY Portfolio'!E12</f>
+        <v>Mr Cooper Group Inc</v>
+      </c>
+      <c r="B9" s="154">
+        <f>'BUY Portfolio'!F12*100</f>
+        <v>3.9</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>'BUY Portfolio'!E13</f>
+        <v>Providence Service Corp/The</v>
+      </c>
+      <c r="B10" s="154">
+        <f>'BUY Portfolio'!F13*100</f>
+        <v>3.6999999999999997</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>'BUY Portfolio'!E14</f>
+        <v>Masimo Corp</v>
+      </c>
+      <c r="B11" s="154">
+        <f>'BUY Portfolio'!F14*100</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>